<commit_message>
added functionality to skip duplicate orders when inserting details
</commit_message>
<xml_diff>
--- a/botlworld.xlsx
+++ b/botlworld.xlsx
@@ -2,14 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-103" yWindow="-103" windowWidth="24892" windowHeight="14914" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Order_Details" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -49,7 +50,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -412,13 +413,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C38"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.6"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -438,569 +439,212 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>087580</t>
-        </is>
+      <c r="A2" t="n">
+        <v>85085</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>18-01-2026</t>
+          <t>19-01-2026</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>11:08 PM</t>
+          <t>01:50 AM</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>085085</t>
-        </is>
+      <c r="A3" t="n">
+        <v>85245</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>18-01-2026</t>
+          <t>19-01-2026</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>11:08 PM</t>
+          <t>01:50 AM</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>085245</t>
-        </is>
+      <c r="A4" t="n">
+        <v>85281</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>18-01-2026</t>
+          <t>19-01-2026</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>11:08 PM</t>
+          <t>01:50 AM</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>085281</t>
-        </is>
+      <c r="A5" t="n">
+        <v>85288</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>18-01-2026</t>
+          <t>19-01-2026</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>11:08 PM</t>
+          <t>01:50 AM</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>085288</t>
-        </is>
+      <c r="A6" t="n">
+        <v>85477</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>18-01-2026</t>
+          <t>19-01-2026</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>11:08 PM</t>
+          <t>01:50 AM</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>085477</t>
-        </is>
+      <c r="A7" t="n">
+        <v>85604</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>18-01-2026</t>
+          <t>19-01-2026</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>11:08 PM</t>
+          <t>01:50 AM</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>87580</v>
+        <v>85629</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>18-01-2026</t>
+          <t>19-01-2026</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>11:11 PM</t>
+          <t>01:50 AM</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>85085</v>
+        <v>85714</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>18-01-2026</t>
+          <t>19-01-2026</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>11:11 PM</t>
+          <t>01:50 AM</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>85245</v>
+        <v>85773</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>18-01-2026</t>
+          <t>19-01-2026</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>11:11 PM</t>
+          <t>01:50 AM</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>85281</v>
+        <v>85811</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>18-01-2026</t>
+          <t>19-01-2026</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>11:11 PM</t>
+          <t>01:50 AM</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>85288</v>
+        <v>85847</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>18-01-2026</t>
+          <t>19-01-2026</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>11:11 PM</t>
+          <t>01:50 AM</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>85477</v>
+        <v>87580</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>18-01-2026</t>
+          <t>19-01-2026</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>11:11 PM</t>
+          <t>01:50 AM</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>87580</v>
+        <v>87581</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>18-01-2026</t>
+          <t>19-01-2026</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>11:37 PM</t>
+          <t>01:53 AM</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>85085</v>
+        <v>84532</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>18-01-2026</t>
+          <t>19-01-2026</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>11:37 PM</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="n">
-        <v>85245</v>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>18-01-2026</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>11:37 PM</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="n">
-        <v>85281</v>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>18-01-2026</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>11:37 PM</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="n">
-        <v>85288</v>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>18-01-2026</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>11:37 PM</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="n">
-        <v>85477</v>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>18-01-2026</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>11:37 PM</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="n">
-        <v>87580</v>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>18-01-2026</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>11:39 PM</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="n">
-        <v>85085</v>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>18-01-2026</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>11:39 PM</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="n">
-        <v>85245</v>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>18-01-2026</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>11:39 PM</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="n">
-        <v>85281</v>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>18-01-2026</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>11:39 PM</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="n">
-        <v>85288</v>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>18-01-2026</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>11:39 PM</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="n">
-        <v>85477</v>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>18-01-2026</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>11:39 PM</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="n">
-        <v>85604</v>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>18-01-2026</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>11:51 PM</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="n">
-        <v>85629</v>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>18-01-2026</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>11:51 PM</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="n">
-        <v>85714</v>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>18-01-2026</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>11:51 PM</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="n">
-        <v>85773</v>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>18-01-2026</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>11:51 PM</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="n">
-        <v>85811</v>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>18-01-2026</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>11:51 PM</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="n">
-        <v>85847</v>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>18-01-2026</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>11:51 PM</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="n">
-        <v>87580</v>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>18-01-2026</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>11:51 PM</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="n">
-        <v>85085</v>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>18-01-2026</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>11:51 PM</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="n">
-        <v>85245</v>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>18-01-2026</t>
-        </is>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>11:51 PM</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="n">
-        <v>85281</v>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>18-01-2026</t>
-        </is>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>11:51 PM</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="n">
-        <v>85288</v>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>18-01-2026</t>
-        </is>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>11:51 PM</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="n">
-        <v>85477</v>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>18-01-2026</t>
-        </is>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>11:51 PM</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="n">
-        <v>87580</v>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>18-01-2026</t>
-        </is>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>11:52 PM</t>
+          <t>01:53 AM</t>
         </is>
       </c>
     </row>

</xml_diff>